<commit_message>
delete and update function
</commit_message>
<xml_diff>
--- a/client/drafts.xlsx
+++ b/client/drafts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1980" windowWidth="25380" windowHeight="13620" tabRatio="500"/>
+    <workbookView xWindow="2600" yWindow="3500" windowWidth="25380" windowHeight="13620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
     <t>db.princesses.insert({ princessName: 'Moana', favRest: { restName: 'Coconuts' , priceRange: '$$$', cuisine: 'Seafood', description: 'Chill, beachy hangout on the Intracoastal dishing seafood &amp; Sunday brunch while yachts cruise by.', rating: 4}, princessReview: 'The best way to destroy Kakamora Coconut Monsters is to eat them all!', imageURL: './images/mo3.png'  })</t>
   </si>
   <si>
-    <t>db.princesses.insert({ princessName: 'Rapunzel', favRest: { restName: 'Hazelnut Soup Cafe' , priceRange: '$$', cuisine: 'Soup', description: 'This is a fictional café that only serves 1 item: Rapunzel's favorite hazelnut soup.', rating: 5}, princessReview: 'Give me more hazelnut soup, or I will never let you use my hair, again!', imageURL: './images/r2.png'  })</t>
+    <t>db.princesses.insert({ princessName: 'Rapunzel', favRest: { restName: 'Hazelnut Soup Cafe' , priceRange: '$$', cuisine: 'Soup', description: "This is a fictional café that only serves 1 item: Rapunzel's favorite hazelnut soup.", rating: 5}, princessReview: 'Give me more hazelnut soup, or I will never let you use my hair, again!', imageURL: './images/r2.png'  })</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>